<commit_message>
Close origin:sell all => not sell, calc AccountValue.
</commit_message>
<xml_diff>
--- a/交易記錄.xlsx
+++ b/交易記錄.xlsx
@@ -27837,22 +27837,22 @@
         <v>951.2952536897914</v>
       </c>
       <c r="E806" t="n">
-        <v>0.9512952536897914</v>
+        <v>0</v>
       </c>
       <c r="F806" t="n">
-        <v>9726.492020124873</v>
+        <v>10678.73856906835</v>
       </c>
       <c r="G806" t="n">
         <v>0</v>
       </c>
       <c r="H806" t="n">
-        <v>9726.492020124873</v>
+        <v>9729.296577246108</v>
       </c>
       <c r="I806" t="n">
-        <v>0</v>
+        <v>7912.016598518725</v>
       </c>
       <c r="J806" t="n">
-        <v>0</v>
+        <v>-1.853261867544388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>